<commit_message>
modified all data to facilitate df import
</commit_message>
<xml_diff>
--- a/data/death_causes.xlsx
+++ b/data/death_causes.xlsx
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="dth00160_" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="dth00160_1" localSheetId="0">Sheet1!#REF!</definedName>
-    <definedName name="emc120000_" localSheetId="0">Sheet1!$A$1:$J$116</definedName>
+    <definedName name="emc120000_" localSheetId="0">Sheet1!$A$1:$J$119</definedName>
     <definedName name="mc360000_" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -81,9 +81,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Death rates</t>
-  </si>
-  <si>
     <t>tuberculosis_deaths</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>suicide_deaths</t>
+  </si>
+  <si>
+    <t>deaths</t>
   </si>
 </sst>
 </file>
@@ -427,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J116"/>
+  <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P13" sqref="O13:P13"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="N110" sqref="N110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,31 +453,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1922,2241 +1922,2256 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1947</v>
-      </c>
-      <c r="B47">
-        <v>1457.4</v>
-      </c>
-      <c r="C47">
-        <v>187.2</v>
-      </c>
-      <c r="D47">
-        <v>69</v>
-      </c>
-      <c r="E47">
-        <v>62.2</v>
-      </c>
-      <c r="F47">
-        <v>129.4</v>
-      </c>
-      <c r="G47">
-        <v>130.1</v>
-      </c>
-      <c r="H47">
-        <v>100.3</v>
-      </c>
-      <c r="I47">
-        <v>49.3</v>
-      </c>
-      <c r="J47">
-        <v>15.7</v>
+        <v>1944</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>1948</v>
-      </c>
-      <c r="B48">
-        <v>1188.2</v>
-      </c>
-      <c r="C48">
-        <v>179.9</v>
-      </c>
-      <c r="D48">
-        <v>70.8</v>
-      </c>
-      <c r="E48">
-        <v>61.3</v>
-      </c>
-      <c r="F48">
-        <v>117.9</v>
-      </c>
-      <c r="G48">
-        <v>66.2</v>
-      </c>
-      <c r="H48">
-        <v>79.5</v>
-      </c>
-      <c r="I48">
-        <v>48.7</v>
-      </c>
-      <c r="J48">
-        <v>15.9</v>
+        <v>1945</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>1949</v>
-      </c>
-      <c r="B49">
-        <v>1156.2</v>
-      </c>
-      <c r="C49">
-        <v>168.9</v>
-      </c>
-      <c r="D49">
-        <v>73.2</v>
-      </c>
-      <c r="E49">
-        <v>64.5</v>
-      </c>
-      <c r="F49">
-        <v>122.6</v>
-      </c>
-      <c r="G49">
-        <v>68.7</v>
-      </c>
-      <c r="H49">
-        <v>80.2</v>
-      </c>
-      <c r="I49">
-        <v>41.9</v>
-      </c>
-      <c r="J49">
-        <v>17.399999999999999</v>
+        <v>1946</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="B50">
-        <v>1087.5999999999999</v>
+        <v>1457.4</v>
       </c>
       <c r="C50">
-        <v>146.4</v>
+        <v>187.2</v>
       </c>
       <c r="D50">
-        <v>77.400000000000006</v>
+        <v>69</v>
       </c>
       <c r="E50">
-        <v>64.2</v>
+        <v>62.2</v>
       </c>
       <c r="F50">
-        <v>127.1</v>
+        <v>129.4</v>
       </c>
       <c r="G50">
-        <v>65.099999999999994</v>
+        <v>130.1</v>
       </c>
       <c r="H50">
-        <v>70.2</v>
+        <v>100.3</v>
       </c>
       <c r="I50">
-        <v>39.5</v>
+        <v>49.3</v>
       </c>
       <c r="J50">
-        <v>19.600000000000001</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>1951</v>
+        <v>1948</v>
       </c>
       <c r="B51">
-        <v>992</v>
+        <v>1188.2</v>
       </c>
       <c r="C51">
-        <v>110.3</v>
+        <v>179.9</v>
       </c>
       <c r="D51">
-        <v>78.5</v>
+        <v>70.8</v>
       </c>
       <c r="E51">
-        <v>63.6</v>
+        <v>61.3</v>
       </c>
       <c r="F51">
-        <v>125.2</v>
+        <v>117.9</v>
       </c>
       <c r="G51">
-        <v>59.8</v>
+        <v>66.2</v>
       </c>
       <c r="H51">
-        <v>70.7</v>
+        <v>79.5</v>
       </c>
       <c r="I51">
-        <v>37.799999999999997</v>
+        <v>48.7</v>
       </c>
       <c r="J51">
-        <v>18.2</v>
+        <v>15.9</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>1952</v>
+        <v>1949</v>
       </c>
       <c r="B52">
-        <v>891.1</v>
+        <v>1156.2</v>
       </c>
       <c r="C52">
-        <v>82.2</v>
+        <v>168.9</v>
       </c>
       <c r="D52">
-        <v>80.900000000000006</v>
+        <v>73.2</v>
       </c>
       <c r="E52">
-        <v>61.3</v>
+        <v>64.5</v>
       </c>
       <c r="F52">
-        <v>128.5</v>
+        <v>122.6</v>
       </c>
       <c r="G52">
-        <v>49.9</v>
+        <v>68.7</v>
       </c>
       <c r="H52">
-        <v>69.3</v>
+        <v>80.2</v>
       </c>
       <c r="I52">
-        <v>36.4</v>
+        <v>41.9</v>
       </c>
       <c r="J52">
-        <v>18.399999999999999</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1953</v>
+        <v>1950</v>
       </c>
       <c r="B53">
-        <v>887.6</v>
+        <v>1087.5999999999999</v>
       </c>
       <c r="C53">
-        <v>66.5</v>
+        <v>146.4</v>
       </c>
       <c r="D53">
-        <v>82.2</v>
+        <v>77.400000000000006</v>
       </c>
       <c r="E53">
-        <v>64.900000000000006</v>
+        <v>64.2</v>
       </c>
       <c r="F53">
-        <v>133.69999999999999</v>
+        <v>127.1</v>
       </c>
       <c r="G53">
-        <v>53.7</v>
+        <v>65.099999999999994</v>
       </c>
       <c r="H53">
-        <v>77.599999999999994</v>
+        <v>70.2</v>
       </c>
       <c r="I53">
-        <v>39.299999999999997</v>
+        <v>39.5</v>
       </c>
       <c r="J53">
-        <v>20.399999999999999</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>1954</v>
+        <v>1951</v>
       </c>
       <c r="B54">
-        <v>817.2</v>
+        <v>992</v>
       </c>
       <c r="C54">
-        <v>62.4</v>
+        <v>110.3</v>
       </c>
       <c r="D54">
-        <v>85.3</v>
+        <v>78.5</v>
       </c>
       <c r="E54">
-        <v>60.2</v>
+        <v>63.6</v>
       </c>
       <c r="F54">
-        <v>132.4</v>
+        <v>125.2</v>
       </c>
       <c r="G54">
-        <v>42.7</v>
+        <v>59.8</v>
       </c>
       <c r="H54">
-        <v>69.5</v>
+        <v>70.7</v>
       </c>
       <c r="I54">
-        <v>39.4</v>
+        <v>37.799999999999997</v>
       </c>
       <c r="J54">
-        <v>23.4</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="B55">
-        <v>776.8</v>
+        <v>891.1</v>
       </c>
       <c r="C55">
-        <v>52.3</v>
+        <v>82.2</v>
       </c>
       <c r="D55">
-        <v>87.1</v>
+        <v>80.900000000000006</v>
       </c>
       <c r="E55">
-        <v>60.9</v>
+        <v>61.3</v>
       </c>
       <c r="F55">
-        <v>136.1</v>
+        <v>128.5</v>
       </c>
       <c r="G55">
-        <v>38.4</v>
+        <v>49.9</v>
       </c>
       <c r="H55">
-        <v>67.099999999999994</v>
+        <v>69.3</v>
       </c>
       <c r="I55">
-        <v>37.299999999999997</v>
+        <v>36.4</v>
       </c>
       <c r="J55">
-        <v>25.2</v>
+        <v>18.399999999999999</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="B56">
-        <v>802.6</v>
+        <v>887.6</v>
       </c>
       <c r="C56">
-        <v>48.6</v>
+        <v>66.5</v>
       </c>
       <c r="D56">
-        <v>90.7</v>
+        <v>82.2</v>
       </c>
       <c r="E56">
-        <v>66</v>
+        <v>64.900000000000006</v>
       </c>
       <c r="F56">
-        <v>148.4</v>
+        <v>133.69999999999999</v>
       </c>
       <c r="G56">
-        <v>38.6</v>
+        <v>53.7</v>
       </c>
       <c r="H56">
-        <v>75.8</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="I56">
-        <v>36.799999999999997</v>
+        <v>39.299999999999997</v>
       </c>
       <c r="J56">
-        <v>24.5</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="B57">
-        <v>826.1</v>
+        <v>817.2</v>
       </c>
       <c r="C57">
-        <v>46.9</v>
+        <v>62.4</v>
       </c>
       <c r="D57">
-        <v>91.3</v>
+        <v>85.3</v>
       </c>
       <c r="E57">
-        <v>73.099999999999994</v>
+        <v>60.2</v>
       </c>
       <c r="F57">
-        <v>151.69999999999999</v>
+        <v>132.4</v>
       </c>
       <c r="G57">
-        <v>48</v>
+        <v>42.7</v>
       </c>
       <c r="H57">
-        <v>80.5</v>
+        <v>69.5</v>
       </c>
       <c r="I57">
-        <v>37.9</v>
+        <v>39.4</v>
       </c>
       <c r="J57">
-        <v>24.3</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>1958</v>
+        <v>1955</v>
       </c>
       <c r="B58">
-        <v>743.6</v>
+        <v>776.8</v>
       </c>
       <c r="C58">
-        <v>39.4</v>
+        <v>52.3</v>
       </c>
       <c r="D58">
-        <v>95.5</v>
+        <v>87.1</v>
       </c>
       <c r="E58">
-        <v>64.8</v>
+        <v>60.9</v>
       </c>
       <c r="F58">
-        <v>148.6</v>
+        <v>136.1</v>
       </c>
       <c r="G58">
-        <v>38.299999999999997</v>
+        <v>38.4</v>
       </c>
       <c r="H58">
-        <v>55.5</v>
+        <v>67.099999999999994</v>
       </c>
       <c r="I58">
-        <v>38.9</v>
+        <v>37.299999999999997</v>
       </c>
       <c r="J58">
-        <v>25.7</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>1959</v>
+        <v>1956</v>
       </c>
       <c r="B59">
-        <v>742.1</v>
+        <v>802.6</v>
       </c>
       <c r="C59">
-        <v>35.5</v>
+        <v>48.6</v>
       </c>
       <c r="D59">
-        <v>98.2</v>
+        <v>90.7</v>
       </c>
       <c r="E59">
-        <v>67.7</v>
+        <v>66</v>
       </c>
       <c r="F59">
-        <v>153.69999999999999</v>
+        <v>148.4</v>
       </c>
       <c r="G59">
+        <v>38.6</v>
+      </c>
+      <c r="H59">
+        <v>75.8</v>
+      </c>
+      <c r="I59">
         <v>36.799999999999997</v>
       </c>
-      <c r="H59">
-        <v>56.7</v>
-      </c>
-      <c r="I59">
-        <v>44.8</v>
-      </c>
       <c r="J59">
-        <v>22.7</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>1960</v>
+        <v>1957</v>
       </c>
       <c r="B60">
-        <v>756.4</v>
+        <v>826.1</v>
       </c>
       <c r="C60">
-        <v>34.200000000000003</v>
+        <v>46.9</v>
       </c>
       <c r="D60">
-        <v>100.4</v>
+        <v>91.3</v>
       </c>
       <c r="E60">
-        <v>73.2</v>
+        <v>73.099999999999994</v>
       </c>
       <c r="F60">
-        <v>160.69999999999999</v>
+        <v>151.69999999999999</v>
       </c>
       <c r="G60">
-        <v>40.200000000000003</v>
+        <v>48</v>
       </c>
       <c r="H60">
-        <v>58</v>
+        <v>80.5</v>
       </c>
       <c r="I60">
-        <v>41.7</v>
+        <v>37.9</v>
       </c>
       <c r="J60">
-        <v>21.6</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>1961</v>
+        <v>1958</v>
       </c>
       <c r="B61">
-        <v>737.8</v>
+        <v>743.6</v>
       </c>
       <c r="C61">
-        <v>29.6</v>
+        <v>39.4</v>
       </c>
       <c r="D61">
-        <v>102.3</v>
+        <v>95.5</v>
       </c>
       <c r="E61">
-        <v>72.099999999999994</v>
+        <v>64.8</v>
       </c>
       <c r="F61">
-        <v>165.4</v>
+        <v>148.6</v>
       </c>
       <c r="G61">
-        <v>33.799999999999997</v>
+        <v>38.299999999999997</v>
       </c>
       <c r="H61">
-        <v>58.2</v>
+        <v>55.5</v>
       </c>
       <c r="I61">
-        <v>44.1</v>
+        <v>38.9</v>
       </c>
       <c r="J61">
-        <v>19.600000000000001</v>
+        <v>25.7</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>1962</v>
+        <v>1959</v>
       </c>
       <c r="B62">
-        <v>746.2</v>
+        <v>742.1</v>
       </c>
       <c r="C62">
-        <v>29.3</v>
+        <v>35.5</v>
       </c>
       <c r="D62">
-        <v>103.2</v>
+        <v>98.2</v>
       </c>
       <c r="E62">
-        <v>76.2</v>
+        <v>67.7</v>
       </c>
       <c r="F62">
-        <v>169.4</v>
+        <v>153.69999999999999</v>
       </c>
       <c r="G62">
-        <v>36.6</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="H62">
-        <v>57.5</v>
+        <v>56.7</v>
       </c>
       <c r="I62">
-        <v>40.299999999999997</v>
+        <v>44.8</v>
       </c>
       <c r="J62">
-        <v>17.600000000000001</v>
+        <v>22.7</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>1963</v>
+        <v>1960</v>
       </c>
       <c r="B63">
-        <v>697.6</v>
+        <v>756.4</v>
       </c>
       <c r="C63">
-        <v>24.2</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="D63">
-        <v>105.5</v>
+        <v>100.4</v>
       </c>
       <c r="E63">
-        <v>70.400000000000006</v>
+        <v>73.2</v>
       </c>
       <c r="F63">
-        <v>171.4</v>
+        <v>160.69999999999999</v>
       </c>
       <c r="G63">
-        <v>27.2</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="H63">
-        <v>50.4</v>
+        <v>58</v>
       </c>
       <c r="I63">
-        <v>41.3</v>
+        <v>41.7</v>
       </c>
       <c r="J63">
-        <v>16.100000000000001</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>1964</v>
+        <v>1961</v>
       </c>
       <c r="B64">
-        <v>692.6</v>
+        <v>737.8</v>
       </c>
       <c r="C64">
-        <v>23.6</v>
+        <v>29.6</v>
       </c>
       <c r="D64">
-        <v>107.3</v>
+        <v>102.3</v>
       </c>
       <c r="E64">
-        <v>70.3</v>
+        <v>72.099999999999994</v>
       </c>
       <c r="F64">
-        <v>171.7</v>
+        <v>165.4</v>
       </c>
       <c r="G64">
-        <v>26.3</v>
+        <v>33.799999999999997</v>
       </c>
       <c r="H64">
-        <v>48.4</v>
+        <v>58.2</v>
       </c>
       <c r="I64">
-        <v>41.6</v>
+        <v>44.1</v>
       </c>
       <c r="J64">
-        <v>15.1</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>1965</v>
+        <v>1962</v>
       </c>
       <c r="B65">
-        <v>712.7</v>
+        <v>746.2</v>
       </c>
       <c r="C65">
-        <v>22.8</v>
+        <v>29.3</v>
       </c>
       <c r="D65">
-        <v>108.4</v>
+        <v>103.2</v>
       </c>
       <c r="E65">
-        <v>77</v>
+        <v>76.2</v>
       </c>
       <c r="F65">
-        <v>175.8</v>
+        <v>169.4</v>
       </c>
       <c r="G65">
-        <v>30.4</v>
+        <v>36.6</v>
       </c>
       <c r="H65">
-        <v>50</v>
+        <v>57.5</v>
       </c>
       <c r="I65">
-        <v>40.9</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="J65">
-        <v>14.7</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>1966</v>
+        <v>1963</v>
       </c>
       <c r="B66">
-        <v>676.7</v>
+        <v>697.6</v>
       </c>
       <c r="C66">
-        <v>20.3</v>
+        <v>24.2</v>
       </c>
       <c r="D66">
-        <v>110.9</v>
+        <v>105.5</v>
       </c>
       <c r="E66">
-        <v>71.900000000000006</v>
+        <v>70.400000000000006</v>
       </c>
       <c r="F66">
-        <v>173.8</v>
+        <v>171.4</v>
       </c>
       <c r="G66">
-        <v>22.9</v>
+        <v>27.2</v>
       </c>
       <c r="H66">
-        <v>44.6</v>
+        <v>50.4</v>
       </c>
       <c r="I66">
-        <v>43</v>
+        <v>41.3</v>
       </c>
       <c r="J66">
-        <v>15.2</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>1967</v>
+        <v>1964</v>
       </c>
       <c r="B67">
-        <v>677.5</v>
+        <v>692.6</v>
       </c>
       <c r="C67">
-        <v>17.8</v>
+        <v>23.6</v>
       </c>
       <c r="D67">
-        <v>113</v>
+        <v>107.3</v>
       </c>
       <c r="E67">
-        <v>75.7</v>
+        <v>70.3</v>
       </c>
       <c r="F67">
-        <v>173.1</v>
+        <v>171.7</v>
       </c>
       <c r="G67">
-        <v>23.5</v>
+        <v>26.3</v>
       </c>
       <c r="H67">
-        <v>43.3</v>
+        <v>48.4</v>
       </c>
       <c r="I67">
-        <v>41.9</v>
+        <v>41.6</v>
       </c>
       <c r="J67">
-        <v>14.2</v>
+        <v>15.1</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>1968</v>
+        <v>1965</v>
       </c>
       <c r="B68">
-        <v>681.1</v>
+        <v>712.7</v>
       </c>
       <c r="C68">
-        <v>16.8</v>
+        <v>22.8</v>
       </c>
       <c r="D68">
-        <v>114.6</v>
+        <v>108.4</v>
       </c>
       <c r="E68">
-        <v>80.2</v>
+        <v>77</v>
       </c>
       <c r="F68">
-        <v>173.5</v>
+        <v>175.8</v>
       </c>
       <c r="G68">
-        <v>25</v>
+        <v>30.4</v>
       </c>
       <c r="H68">
-        <v>39.4</v>
+        <v>50</v>
       </c>
       <c r="I68">
-        <v>40.200000000000003</v>
+        <v>40.9</v>
       </c>
       <c r="J68">
-        <v>14.5</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>1969</v>
+        <v>1966</v>
       </c>
       <c r="B69">
-        <v>680</v>
+        <v>676.7</v>
       </c>
       <c r="C69">
-        <v>16.100000000000001</v>
+        <v>20.3</v>
       </c>
       <c r="D69">
-        <v>116.2</v>
+        <v>110.9</v>
       </c>
       <c r="E69">
-        <v>81.7</v>
+        <v>71.900000000000006</v>
       </c>
       <c r="F69">
-        <v>174.4</v>
+        <v>173.8</v>
       </c>
       <c r="G69">
-        <v>24.9</v>
+        <v>22.9</v>
       </c>
       <c r="H69">
-        <v>37.1</v>
+        <v>44.6</v>
       </c>
       <c r="I69">
-        <v>42.2</v>
+        <v>43</v>
       </c>
       <c r="J69">
-        <v>14.5</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>1970</v>
+        <v>1967</v>
       </c>
       <c r="B70">
-        <v>691.4</v>
+        <v>677.5</v>
       </c>
       <c r="C70">
-        <v>15.4</v>
+        <v>17.8</v>
       </c>
       <c r="D70">
-        <v>116.3</v>
+        <v>113</v>
       </c>
       <c r="E70">
-        <v>86.7</v>
+        <v>75.7</v>
       </c>
       <c r="F70">
-        <v>175.8</v>
+        <v>173.1</v>
       </c>
       <c r="G70">
-        <v>27.1</v>
+        <v>23.5</v>
       </c>
       <c r="H70">
-        <v>38.1</v>
+        <v>43.3</v>
       </c>
       <c r="I70">
-        <v>42.5</v>
+        <v>41.9</v>
       </c>
       <c r="J70">
-        <v>15.3</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>1971</v>
+        <v>1968</v>
       </c>
       <c r="B71">
-        <v>656</v>
+        <v>681.1</v>
       </c>
       <c r="C71">
-        <v>13</v>
+        <v>16.8</v>
       </c>
       <c r="D71">
-        <v>117.7</v>
+        <v>114.6</v>
       </c>
       <c r="E71">
-        <v>82</v>
+        <v>80.2</v>
       </c>
       <c r="F71">
-        <v>169.6</v>
+        <v>173.5</v>
       </c>
       <c r="G71">
-        <v>22.1</v>
+        <v>25</v>
       </c>
       <c r="H71">
-        <v>34</v>
+        <v>39.4</v>
       </c>
       <c r="I71">
-        <v>40.700000000000003</v>
+        <v>40.200000000000003</v>
       </c>
       <c r="J71">
-        <v>15.6</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>1972</v>
+        <v>1969</v>
       </c>
       <c r="B72">
-        <v>646.6</v>
+        <v>680</v>
       </c>
       <c r="C72">
-        <v>11.9</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="D72">
-        <v>120.4</v>
+        <v>116.2</v>
       </c>
       <c r="E72">
-        <v>81.2</v>
+        <v>81.7</v>
       </c>
       <c r="F72">
-        <v>166.7</v>
+        <v>174.4</v>
       </c>
       <c r="G72">
-        <v>21.9</v>
+        <v>24.9</v>
       </c>
       <c r="H72">
-        <v>30.8</v>
+        <v>37.1</v>
       </c>
       <c r="I72">
-        <v>40.1</v>
+        <v>42.2</v>
       </c>
       <c r="J72">
-        <v>17</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>1973</v>
+        <v>1970</v>
       </c>
       <c r="B73">
-        <v>656.4</v>
+        <v>691.4</v>
       </c>
       <c r="C73">
-        <v>11.1</v>
+        <v>15.4</v>
       </c>
       <c r="D73">
-        <v>121.2</v>
+        <v>116.3</v>
       </c>
       <c r="E73">
-        <v>87.3</v>
+        <v>86.7</v>
       </c>
       <c r="F73">
-        <v>166.9</v>
+        <v>175.8</v>
       </c>
       <c r="G73">
-        <v>25</v>
+        <v>27.1</v>
       </c>
       <c r="H73">
-        <v>30.9</v>
+        <v>38.1</v>
       </c>
       <c r="I73">
-        <v>37.200000000000003</v>
+        <v>42.5</v>
       </c>
       <c r="J73">
-        <v>17.399999999999999</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>1974</v>
+        <v>1971</v>
       </c>
       <c r="B74">
-        <v>649.4</v>
+        <v>656</v>
       </c>
       <c r="C74">
-        <v>10.4</v>
+        <v>13</v>
       </c>
       <c r="D74">
-        <v>122.2</v>
+        <v>117.7</v>
       </c>
       <c r="E74">
-        <v>89.8</v>
+        <v>82</v>
       </c>
       <c r="F74">
-        <v>163</v>
+        <v>169.6</v>
       </c>
       <c r="G74">
-        <v>26.1</v>
+        <v>22.1</v>
       </c>
       <c r="H74">
-        <v>29.7</v>
+        <v>34</v>
       </c>
       <c r="I74">
-        <v>33</v>
+        <v>40.700000000000003</v>
       </c>
       <c r="J74">
-        <v>17.5</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>1975</v>
+        <v>1972</v>
       </c>
       <c r="B75">
-        <v>631.20000000000005</v>
+        <v>646.6</v>
       </c>
       <c r="C75">
-        <v>9.5</v>
+        <v>11.9</v>
       </c>
       <c r="D75">
-        <v>122.6</v>
+        <v>120.4</v>
       </c>
       <c r="E75">
-        <v>89.2</v>
+        <v>81.2</v>
       </c>
       <c r="F75">
-        <v>156.69999999999999</v>
+        <v>166.7</v>
       </c>
       <c r="G75">
-        <v>27.4</v>
+        <v>21.9</v>
       </c>
       <c r="H75">
-        <v>26.9</v>
+        <v>30.8</v>
       </c>
       <c r="I75">
-        <v>30.3</v>
+        <v>40.1</v>
       </c>
       <c r="J75">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>1976</v>
+        <v>1973</v>
       </c>
       <c r="B76">
-        <v>625.6</v>
+        <v>656.4</v>
       </c>
       <c r="C76">
-        <v>8.5</v>
+        <v>11.1</v>
       </c>
       <c r="D76">
-        <v>125.3</v>
+        <v>121.2</v>
       </c>
       <c r="E76">
-        <v>92.2</v>
+        <v>87.3</v>
       </c>
       <c r="F76">
-        <v>154.5</v>
+        <v>166.9</v>
       </c>
       <c r="G76">
-        <v>26.6</v>
+        <v>25</v>
       </c>
       <c r="H76">
-        <v>26.4</v>
+        <v>30.9</v>
       </c>
       <c r="I76">
-        <v>28</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="J76">
-        <v>17.600000000000001</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>1977</v>
+        <v>1974</v>
       </c>
       <c r="B77">
-        <v>608</v>
+        <v>649.4</v>
       </c>
       <c r="C77">
-        <v>7.8</v>
+        <v>10.4</v>
       </c>
       <c r="D77">
-        <v>128.4</v>
+        <v>122.2</v>
       </c>
       <c r="E77">
-        <v>91.2</v>
+        <v>89.8</v>
       </c>
       <c r="F77">
-        <v>149.80000000000001</v>
+        <v>163</v>
       </c>
       <c r="G77">
-        <v>23.3</v>
+        <v>26.1</v>
       </c>
       <c r="H77">
-        <v>25</v>
+        <v>29.7</v>
       </c>
       <c r="I77">
-        <v>26.7</v>
+        <v>33</v>
       </c>
       <c r="J77">
-        <v>17.899999999999999</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>1978</v>
+        <v>1975</v>
       </c>
       <c r="B78">
-        <v>607.6</v>
+        <v>631.20000000000005</v>
       </c>
       <c r="C78">
-        <v>7.2</v>
+        <v>9.5</v>
       </c>
       <c r="D78">
-        <v>131.30000000000001</v>
+        <v>122.6</v>
       </c>
       <c r="E78">
-        <v>93.3</v>
+        <v>89.2</v>
       </c>
       <c r="F78">
-        <v>146.19999999999999</v>
+        <v>156.69999999999999</v>
       </c>
       <c r="G78">
-        <v>24.7</v>
+        <v>27.4</v>
       </c>
       <c r="H78">
-        <v>24.4</v>
+        <v>26.9</v>
       </c>
       <c r="I78">
-        <v>26.2</v>
+        <v>30.3</v>
       </c>
       <c r="J78">
-        <v>17.600000000000001</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>1979</v>
+        <v>1976</v>
       </c>
       <c r="B79">
-        <v>597.29999999999995</v>
+        <v>625.6</v>
       </c>
       <c r="C79">
-        <v>5.8</v>
+        <v>8.5</v>
       </c>
       <c r="D79">
-        <v>135.69999999999999</v>
+        <v>125.3</v>
       </c>
       <c r="E79">
-        <v>96.9</v>
+        <v>92.2</v>
       </c>
       <c r="F79">
-        <v>137.69999999999999</v>
+        <v>154.5</v>
       </c>
       <c r="G79">
-        <v>23.7</v>
+        <v>26.6</v>
       </c>
       <c r="H79">
-        <v>25.5</v>
+        <v>26.4</v>
       </c>
       <c r="I79">
-        <v>25.3</v>
+        <v>28</v>
       </c>
       <c r="J79">
-        <v>18</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>1980</v>
+        <v>1977</v>
       </c>
       <c r="B80">
-        <v>621.4</v>
+        <v>608</v>
       </c>
       <c r="C80">
-        <v>5.5</v>
+        <v>7.8</v>
       </c>
       <c r="D80">
-        <v>139.1</v>
+        <v>128.4</v>
       </c>
       <c r="E80">
-        <v>106.2</v>
+        <v>91.2</v>
       </c>
       <c r="F80">
-        <v>139.5</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="G80">
-        <v>28.4</v>
+        <v>23.3</v>
       </c>
       <c r="H80">
-        <v>27.6</v>
+        <v>25</v>
       </c>
       <c r="I80">
-        <v>25.1</v>
+        <v>26.7</v>
       </c>
       <c r="J80">
-        <v>17.7</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>1981</v>
+        <v>1978</v>
       </c>
       <c r="B81">
-        <v>614.5</v>
+        <v>607.6</v>
       </c>
       <c r="C81">
-        <v>4.9000000000000004</v>
+        <v>7.2</v>
       </c>
       <c r="D81">
-        <v>142</v>
+        <v>131.30000000000001</v>
       </c>
       <c r="E81">
-        <v>107.5</v>
+        <v>93.3</v>
       </c>
       <c r="F81">
-        <v>134.30000000000001</v>
+        <v>146.19999999999999</v>
       </c>
       <c r="G81">
-        <v>28.7</v>
+        <v>24.7</v>
       </c>
       <c r="H81">
-        <v>25.5</v>
+        <v>24.4</v>
       </c>
       <c r="I81">
-        <v>24.8</v>
+        <v>26.2</v>
       </c>
       <c r="J81">
-        <v>17.100000000000001</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>1982</v>
+        <v>1979</v>
       </c>
       <c r="B82">
-        <v>603.20000000000005</v>
+        <v>597.29999999999995</v>
       </c>
       <c r="C82">
-        <v>4.5</v>
+        <v>5.8</v>
       </c>
       <c r="D82">
-        <v>144.19999999999999</v>
+        <v>135.69999999999999</v>
       </c>
       <c r="E82">
-        <v>106.7</v>
+        <v>96.9</v>
       </c>
       <c r="F82">
-        <v>125</v>
+        <v>137.69999999999999</v>
       </c>
       <c r="G82">
-        <v>29.9</v>
+        <v>23.7</v>
       </c>
       <c r="H82">
-        <v>23.3</v>
+        <v>25.5</v>
       </c>
       <c r="I82">
-        <v>24.7</v>
+        <v>25.3</v>
       </c>
       <c r="J82">
-        <v>17.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>1983</v>
+        <v>1980</v>
       </c>
       <c r="B83">
-        <v>623</v>
+        <v>621.4</v>
       </c>
       <c r="C83">
-        <v>4.5</v>
+        <v>5.5</v>
       </c>
       <c r="D83">
-        <v>148.30000000000001</v>
+        <v>139.1</v>
       </c>
       <c r="E83">
-        <v>111.3</v>
+        <v>106.2</v>
       </c>
       <c r="F83">
-        <v>122.8</v>
+        <v>139.5</v>
       </c>
       <c r="G83">
-        <v>33.9</v>
+        <v>28.4</v>
       </c>
       <c r="H83">
-        <v>24.7</v>
+        <v>27.6</v>
       </c>
       <c r="I83">
-        <v>25</v>
+        <v>25.1</v>
       </c>
       <c r="J83">
-        <v>21</v>
+        <v>17.7</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>1984</v>
+        <v>1981</v>
       </c>
       <c r="B84">
-        <v>619.29999999999995</v>
+        <v>614.5</v>
       </c>
       <c r="C84">
-        <v>4.0999999999999996</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="D84">
-        <v>152.5</v>
+        <v>142</v>
       </c>
       <c r="E84">
-        <v>113.9</v>
+        <v>107.5</v>
       </c>
       <c r="F84">
-        <v>117.2</v>
+        <v>134.30000000000001</v>
       </c>
       <c r="G84">
-        <v>32.5</v>
+        <v>28.7</v>
       </c>
       <c r="H84">
-        <v>24.1</v>
+        <v>25.5</v>
       </c>
       <c r="I84">
-        <v>24.6</v>
+        <v>24.8</v>
       </c>
       <c r="J84">
-        <v>20.399999999999999</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>1985</v>
+        <v>1982</v>
       </c>
       <c r="B85">
-        <v>625.5</v>
+        <v>603.20000000000005</v>
       </c>
       <c r="C85">
-        <v>3.9</v>
+        <v>4.5</v>
       </c>
       <c r="D85">
-        <v>156.1</v>
+        <v>144.19999999999999</v>
       </c>
       <c r="E85">
-        <v>117.3</v>
+        <v>106.7</v>
       </c>
       <c r="F85">
-        <v>112.2</v>
+        <v>125</v>
       </c>
       <c r="G85">
-        <v>37.5</v>
+        <v>29.9</v>
       </c>
       <c r="H85">
-        <v>23.1</v>
+        <v>23.3</v>
       </c>
       <c r="I85">
-        <v>24.6</v>
+        <v>24.7</v>
       </c>
       <c r="J85">
-        <v>19.399999999999999</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>1986</v>
+        <v>1983</v>
       </c>
       <c r="B86">
-        <v>620.6</v>
+        <v>623</v>
       </c>
       <c r="C86">
-        <v>3.4</v>
+        <v>4.5</v>
       </c>
       <c r="D86">
-        <v>158.5</v>
+        <v>148.30000000000001</v>
       </c>
       <c r="E86">
-        <v>117.9</v>
+        <v>111.3</v>
       </c>
       <c r="F86">
-        <v>106.9</v>
+        <v>122.8</v>
       </c>
       <c r="G86">
-        <v>39.1</v>
+        <v>33.9</v>
       </c>
       <c r="H86">
-        <v>22.2</v>
+        <v>24.7</v>
       </c>
       <c r="I86">
-        <v>23.7</v>
+        <v>25</v>
       </c>
       <c r="J86">
-        <v>21.2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>1987</v>
+        <v>1984</v>
       </c>
       <c r="B87">
-        <v>618.1</v>
+        <v>619.29999999999995</v>
       </c>
       <c r="C87">
-        <v>3.3</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D87">
-        <v>164.2</v>
+        <v>152.5</v>
       </c>
       <c r="E87">
-        <v>118.4</v>
+        <v>113.9</v>
       </c>
       <c r="F87">
-        <v>101.7</v>
+        <v>117.2</v>
       </c>
       <c r="G87">
-        <v>40.299999999999997</v>
+        <v>32.5</v>
       </c>
       <c r="H87">
-        <v>20.8</v>
+        <v>24.1</v>
       </c>
       <c r="I87">
-        <v>23.2</v>
+        <v>24.6</v>
       </c>
       <c r="J87">
-        <v>19.600000000000001</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>1988</v>
+        <v>1985</v>
       </c>
       <c r="B88">
-        <v>649.9</v>
+        <v>625.5</v>
       </c>
       <c r="C88">
-        <v>3.2</v>
+        <v>3.9</v>
       </c>
       <c r="D88">
-        <v>168.4</v>
+        <v>156.1</v>
       </c>
       <c r="E88">
-        <v>129.4</v>
+        <v>117.3</v>
       </c>
       <c r="F88">
-        <v>105.5</v>
+        <v>112.2</v>
       </c>
       <c r="G88">
-        <v>46.8</v>
+        <v>37.5</v>
       </c>
       <c r="H88">
-        <v>21.6</v>
+        <v>23.1</v>
       </c>
       <c r="I88">
-        <v>24.8</v>
+        <v>24.6</v>
       </c>
       <c r="J88">
-        <v>18.7</v>
+        <v>19.399999999999999</v>
       </c>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>1989</v>
+        <v>1986</v>
       </c>
       <c r="B89">
-        <v>644</v>
+        <v>620.6</v>
       </c>
       <c r="C89">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="D89">
-        <v>173.6</v>
+        <v>158.5</v>
       </c>
       <c r="E89">
-        <v>128.1</v>
+        <v>117.9</v>
       </c>
       <c r="F89">
-        <v>98.5</v>
+        <v>106.9</v>
       </c>
       <c r="G89">
-        <v>48.1</v>
+        <v>39.1</v>
       </c>
       <c r="H89">
-        <v>19.399999999999999</v>
+        <v>22.2</v>
       </c>
       <c r="I89">
-        <v>25.4</v>
+        <v>23.7</v>
       </c>
       <c r="J89">
-        <v>17.3</v>
+        <v>21.2</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>1990</v>
+        <v>1987</v>
       </c>
       <c r="B90">
-        <v>668.4</v>
+        <v>618.1</v>
       </c>
       <c r="C90">
-        <v>3</v>
+        <v>3.3</v>
       </c>
       <c r="D90">
-        <v>177.2</v>
+        <v>164.2</v>
       </c>
       <c r="E90">
-        <v>134.80000000000001</v>
+        <v>118.4</v>
       </c>
       <c r="F90">
-        <v>99.4</v>
+        <v>101.7</v>
       </c>
       <c r="G90">
-        <v>55.6</v>
+        <v>40.299999999999997</v>
       </c>
       <c r="H90">
-        <v>19.7</v>
+        <v>20.8</v>
       </c>
       <c r="I90">
-        <v>26.2</v>
+        <v>23.2</v>
       </c>
       <c r="J90">
-        <v>16.399999999999999</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>1991</v>
+        <v>1988</v>
       </c>
       <c r="B91">
-        <v>674.1</v>
+        <v>649.9</v>
       </c>
       <c r="C91">
-        <v>2.7</v>
+        <v>3.2</v>
       </c>
       <c r="D91">
-        <v>181.7</v>
+        <v>168.4</v>
       </c>
       <c r="E91">
-        <v>137.19999999999999</v>
+        <v>129.4</v>
       </c>
       <c r="F91">
-        <v>96.2</v>
+        <v>105.5</v>
       </c>
       <c r="G91">
-        <v>56.9</v>
+        <v>46.8</v>
       </c>
       <c r="H91">
-        <v>18.8</v>
+        <v>21.6</v>
       </c>
       <c r="I91">
-        <v>26.9</v>
+        <v>24.8</v>
       </c>
       <c r="J91">
-        <v>16.100000000000001</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>1992</v>
+        <v>1989</v>
       </c>
       <c r="B92">
-        <v>693.8</v>
+        <v>644</v>
       </c>
       <c r="C92">
-        <v>2.7</v>
+        <v>2.9</v>
       </c>
       <c r="D92">
-        <v>187.8</v>
+        <v>173.6</v>
       </c>
       <c r="E92">
-        <v>142.19999999999999</v>
+        <v>128.1</v>
       </c>
       <c r="F92">
-        <v>95.6</v>
+        <v>98.5</v>
       </c>
       <c r="G92">
-        <v>60.2</v>
+        <v>48.1</v>
       </c>
       <c r="H92">
-        <v>18.899999999999999</v>
+        <v>19.399999999999999</v>
       </c>
       <c r="I92">
-        <v>28.1</v>
+        <v>25.4</v>
       </c>
       <c r="J92">
-        <v>16.899999999999999</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>1993</v>
+        <v>1990</v>
       </c>
       <c r="B93">
-        <v>709.7</v>
+        <v>668.4</v>
       </c>
       <c r="C93">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="D93">
-        <v>190.4</v>
+        <v>177.2</v>
       </c>
       <c r="E93">
-        <v>145.6</v>
+        <v>134.80000000000001</v>
       </c>
       <c r="F93">
-        <v>96</v>
+        <v>99.4</v>
       </c>
       <c r="G93">
-        <v>65.5</v>
+        <v>55.6</v>
       </c>
       <c r="H93">
-        <v>18.7</v>
+        <v>19.7</v>
       </c>
       <c r="I93">
-        <v>28</v>
+        <v>26.2</v>
       </c>
       <c r="J93">
-        <v>16.600000000000001</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="B94">
-        <v>706</v>
+        <v>674.1</v>
       </c>
       <c r="C94">
-        <v>2.5</v>
+        <v>2.7</v>
       </c>
       <c r="D94">
-        <v>196.4</v>
+        <v>181.7</v>
       </c>
       <c r="E94">
-        <v>128.6</v>
+        <v>137.19999999999999</v>
       </c>
       <c r="F94">
-        <v>96.9</v>
+        <v>96.2</v>
       </c>
       <c r="G94">
-        <v>67.2</v>
+        <v>56.9</v>
       </c>
       <c r="H94">
-        <v>18.899999999999999</v>
+        <v>18.8</v>
       </c>
       <c r="I94">
-        <v>29.1</v>
+        <v>26.9</v>
       </c>
       <c r="J94">
-        <v>16.899999999999999</v>
+        <v>16.100000000000001</v>
       </c>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="B95">
-        <v>741.9</v>
+        <v>693.8</v>
       </c>
       <c r="C95">
-        <v>2.6</v>
+        <v>2.7</v>
       </c>
       <c r="D95">
-        <v>211.6</v>
+        <v>187.8</v>
       </c>
       <c r="E95">
-        <v>112</v>
+        <v>142.19999999999999</v>
       </c>
       <c r="F95">
-        <v>117.9</v>
+        <v>95.6</v>
       </c>
       <c r="G95">
-        <v>64.099999999999994</v>
+        <v>60.2</v>
       </c>
       <c r="H95">
-        <v>17.3</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="I95">
-        <v>36.5</v>
+        <v>28.1</v>
       </c>
       <c r="J95">
-        <v>17.2</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="B96">
-        <v>718.6</v>
+        <v>709.7</v>
       </c>
       <c r="C96">
-        <v>2.2999999999999998</v>
+        <v>2.6</v>
       </c>
       <c r="D96">
-        <v>217.5</v>
+        <v>190.4</v>
       </c>
       <c r="E96">
-        <v>110.8</v>
+        <v>145.6</v>
       </c>
       <c r="F96">
-        <v>112.6</v>
+        <v>96</v>
       </c>
       <c r="G96">
-        <v>56.9</v>
+        <v>65.5</v>
       </c>
       <c r="H96">
-        <v>16.7</v>
+        <v>18.7</v>
       </c>
       <c r="I96">
-        <v>31.4</v>
+        <v>28</v>
       </c>
       <c r="J96">
-        <v>17.8</v>
+        <v>16.600000000000001</v>
       </c>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="B97">
-        <v>730.9</v>
+        <v>706</v>
       </c>
       <c r="C97">
-        <v>2.2000000000000002</v>
+        <v>2.5</v>
       </c>
       <c r="D97">
-        <v>220.4</v>
+        <v>196.4</v>
       </c>
       <c r="E97">
-        <v>112.2</v>
+        <v>128.6</v>
       </c>
       <c r="F97">
-        <v>111</v>
+        <v>96.9</v>
       </c>
       <c r="G97">
-        <v>63.1</v>
+        <v>67.2</v>
       </c>
       <c r="H97">
-        <v>17.2</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="I97">
-        <v>31.1</v>
+        <v>29.1</v>
       </c>
       <c r="J97">
-        <v>18.8</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="B98">
-        <v>747.7</v>
+        <v>741.9</v>
       </c>
       <c r="C98">
-        <v>2.2000000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="D98">
-        <v>226.7</v>
+        <v>211.6</v>
       </c>
       <c r="E98">
-        <v>114.3</v>
+        <v>112</v>
       </c>
       <c r="F98">
-        <v>110</v>
+        <v>117.9</v>
       </c>
       <c r="G98">
-        <v>63.8</v>
+        <v>64.099999999999994</v>
       </c>
       <c r="H98">
-        <v>17.100000000000001</v>
+        <v>17.3</v>
       </c>
       <c r="I98">
-        <v>31.1</v>
+        <v>36.5</v>
       </c>
       <c r="J98">
-        <v>25.4</v>
+        <v>17.2</v>
       </c>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="B99">
-        <v>782.9</v>
+        <v>718.6</v>
       </c>
       <c r="C99">
         <v>2.2999999999999998</v>
       </c>
       <c r="D99">
-        <v>231.6</v>
+        <v>217.5</v>
       </c>
       <c r="E99">
-        <v>120.4</v>
+        <v>110.8</v>
       </c>
       <c r="F99">
-        <v>110.8</v>
+        <v>112.6</v>
       </c>
       <c r="G99">
-        <v>74.900000000000006</v>
+        <v>56.9</v>
       </c>
       <c r="H99">
-        <v>18.2</v>
+        <v>16.7</v>
       </c>
       <c r="I99">
-        <v>32</v>
+        <v>31.4</v>
       </c>
       <c r="J99">
-        <v>25</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="B100">
-        <v>765.6</v>
+        <v>730.9</v>
       </c>
       <c r="C100">
-        <v>2.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D100">
-        <v>235.2</v>
+        <v>220.4</v>
       </c>
       <c r="E100">
-        <v>116.8</v>
+        <v>112.2</v>
       </c>
       <c r="F100">
-        <v>105.5</v>
+        <v>111</v>
       </c>
       <c r="G100">
-        <v>69.2</v>
+        <v>63.1</v>
       </c>
       <c r="H100">
-        <v>16.899999999999999</v>
+        <v>17.2</v>
       </c>
       <c r="I100">
-        <v>31.4</v>
+        <v>31.1</v>
       </c>
       <c r="J100">
-        <v>24.1</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="B101">
-        <v>770.7</v>
+        <v>747.7</v>
       </c>
       <c r="C101">
-        <v>2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D101">
-        <v>238.8</v>
+        <v>226.7</v>
       </c>
       <c r="E101">
-        <v>117.8</v>
+        <v>114.3</v>
       </c>
       <c r="F101">
-        <v>104.7</v>
+        <v>110</v>
       </c>
       <c r="G101">
-        <v>67.8</v>
+        <v>63.8</v>
       </c>
       <c r="H101">
-        <v>17.600000000000001</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="I101">
-        <v>31.4</v>
+        <v>31.1</v>
       </c>
       <c r="J101">
-        <v>23.3</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="B102">
-        <v>779.6</v>
+        <v>782.9</v>
       </c>
       <c r="C102">
-        <v>1.8</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D102">
-        <v>241.7</v>
+        <v>231.6</v>
       </c>
       <c r="E102">
-        <v>121</v>
+        <v>120.4</v>
       </c>
       <c r="F102">
-        <v>103.4</v>
+        <v>110.8</v>
       </c>
       <c r="G102">
-        <v>69.400000000000006</v>
+        <v>74.900000000000006</v>
       </c>
       <c r="H102">
-        <v>18</v>
+        <v>18.2</v>
       </c>
       <c r="I102">
-        <v>30.7</v>
+        <v>32</v>
       </c>
       <c r="J102">
-        <v>23.8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="B103">
-        <v>804.6</v>
+        <v>765.6</v>
       </c>
       <c r="C103">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="D103">
-        <v>245.4</v>
+        <v>235.2</v>
       </c>
       <c r="E103">
-        <v>126.5</v>
+        <v>116.8</v>
       </c>
       <c r="F103">
-        <v>104.7</v>
+        <v>105.5</v>
       </c>
       <c r="G103">
-        <v>75.3</v>
+        <v>69.2</v>
       </c>
       <c r="H103">
-        <v>18.600000000000001</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="I103">
-        <v>30.7</v>
+        <v>31.4</v>
       </c>
       <c r="J103">
-        <v>25.5</v>
+        <v>24.1</v>
       </c>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>2004</v>
+        <v>2001</v>
       </c>
       <c r="B104">
-        <v>815.2</v>
+        <v>770.7</v>
       </c>
       <c r="C104">
-        <v>1.8</v>
+        <v>2</v>
       </c>
       <c r="D104">
-        <v>253.9</v>
+        <v>238.8</v>
       </c>
       <c r="E104">
-        <v>126.5</v>
+        <v>117.8</v>
       </c>
       <c r="F104">
-        <v>102.3</v>
+        <v>104.7</v>
       </c>
       <c r="G104">
-        <v>75.7</v>
+        <v>67.8</v>
       </c>
       <c r="H104">
-        <v>19.100000000000001</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="I104">
-        <v>30.3</v>
+        <v>31.4</v>
       </c>
       <c r="J104">
-        <v>24</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>2005</v>
+        <v>2002</v>
       </c>
       <c r="B105">
-        <v>858.8</v>
+        <v>779.6</v>
       </c>
       <c r="C105">
         <v>1.8</v>
       </c>
       <c r="D105">
-        <v>258.3</v>
+        <v>241.7</v>
       </c>
       <c r="E105">
-        <v>137.19999999999999</v>
+        <v>121</v>
       </c>
       <c r="F105">
-        <v>105.3</v>
+        <v>103.4</v>
       </c>
       <c r="G105">
-        <v>85</v>
+        <v>69.400000000000006</v>
       </c>
       <c r="H105">
-        <v>20.9</v>
+        <v>18</v>
       </c>
       <c r="I105">
-        <v>31.6</v>
+        <v>30.7</v>
       </c>
       <c r="J105">
-        <v>24.2</v>
+        <v>23.8</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>2006</v>
+        <v>2003</v>
       </c>
       <c r="B106">
-        <v>859.6</v>
+        <v>804.6</v>
       </c>
       <c r="C106">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="D106">
-        <v>261</v>
+        <v>245.4</v>
       </c>
       <c r="E106">
-        <v>137.19999999999999</v>
+        <v>126.5</v>
       </c>
       <c r="F106">
-        <v>101.7</v>
+        <v>104.7</v>
       </c>
       <c r="G106">
-        <v>85</v>
+        <v>75.3</v>
       </c>
       <c r="H106">
-        <v>22</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="I106">
-        <v>30.3</v>
+        <v>30.7</v>
       </c>
       <c r="J106">
-        <v>23.7</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>2007</v>
+        <v>2004</v>
       </c>
       <c r="B107">
-        <v>879</v>
+        <v>815.2</v>
       </c>
       <c r="C107">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="D107">
-        <v>266.89999999999998</v>
+        <v>253.9</v>
       </c>
       <c r="E107">
-        <v>139.19999999999999</v>
+        <v>126.5</v>
       </c>
       <c r="F107">
-        <v>100.8</v>
+        <v>102.3</v>
       </c>
       <c r="G107">
-        <v>87.4</v>
+        <v>75.7</v>
       </c>
       <c r="H107">
-        <v>24.4</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="I107">
-        <v>30.1</v>
+        <v>30.3</v>
       </c>
       <c r="J107">
-        <v>24.4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>2008</v>
+        <v>2005</v>
       </c>
       <c r="B108">
-        <v>907.1</v>
+        <v>858.8</v>
       </c>
       <c r="C108">
         <v>1.8</v>
       </c>
       <c r="D108">
-        <v>272.3</v>
+        <v>258.3</v>
       </c>
       <c r="E108">
-        <v>144.4</v>
+        <v>137.19999999999999</v>
       </c>
       <c r="F108">
-        <v>100.9</v>
+        <v>105.3</v>
       </c>
       <c r="G108">
-        <v>91.6</v>
+        <v>85</v>
       </c>
       <c r="H108">
-        <v>28.6</v>
+        <v>20.9</v>
       </c>
       <c r="I108">
-        <v>30.3</v>
+        <v>31.6</v>
       </c>
       <c r="J108">
-        <v>24</v>
+        <v>24.2</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="B109">
-        <v>907.5</v>
+        <v>859.6</v>
       </c>
       <c r="C109">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="D109">
-        <v>273.5</v>
+        <v>261</v>
       </c>
       <c r="E109">
-        <v>143.69999999999999</v>
+        <v>137.19999999999999</v>
       </c>
       <c r="F109">
-        <v>97.2</v>
+        <v>101.7</v>
       </c>
       <c r="G109">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H109">
-        <v>30.7</v>
+        <v>22</v>
       </c>
       <c r="I109">
-        <v>30</v>
+        <v>30.3</v>
       </c>
       <c r="J109">
-        <v>24.4</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>2010</v>
+        <v>2007</v>
       </c>
       <c r="B110">
-        <v>947.1</v>
+        <v>879</v>
       </c>
       <c r="C110">
         <v>1.7</v>
       </c>
       <c r="D110">
-        <v>279.7</v>
+        <v>266.89999999999998</v>
       </c>
       <c r="E110">
-        <v>149.80000000000001</v>
+        <v>139.19999999999999</v>
       </c>
       <c r="F110">
-        <v>97.7</v>
+        <v>100.8</v>
       </c>
       <c r="G110">
-        <v>94.1</v>
+        <v>87.4</v>
       </c>
       <c r="H110">
-        <v>35.9</v>
+        <v>24.4</v>
       </c>
       <c r="I110">
-        <v>32.200000000000003</v>
+        <v>30.1</v>
       </c>
       <c r="J110">
-        <v>23.4</v>
+        <v>24.4</v>
       </c>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>2011</v>
+        <v>2008</v>
       </c>
       <c r="B111">
-        <v>993.1</v>
+        <v>907.1</v>
       </c>
       <c r="C111">
-        <v>1.7</v>
+        <v>1.8</v>
       </c>
       <c r="D111">
-        <v>283.2</v>
+        <v>272.3</v>
       </c>
       <c r="E111">
-        <v>154.5</v>
+        <v>144.4</v>
       </c>
       <c r="F111">
-        <v>98.2</v>
+        <v>100.9</v>
       </c>
       <c r="G111">
-        <v>98.9</v>
+        <v>91.6</v>
       </c>
       <c r="H111">
-        <v>41.4</v>
+        <v>28.6</v>
       </c>
       <c r="I111">
-        <v>47.1</v>
+        <v>30.3</v>
       </c>
       <c r="J111">
-        <v>22.9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>2012</v>
+        <v>2009</v>
       </c>
       <c r="B112">
-        <v>997.5</v>
+        <v>907.5</v>
       </c>
       <c r="C112">
         <v>1.7</v>
       </c>
       <c r="D112">
-        <v>286.60000000000002</v>
+        <v>273.5</v>
       </c>
       <c r="E112">
-        <v>157.9</v>
+        <v>143.69999999999999</v>
       </c>
       <c r="F112">
-        <v>96.5</v>
+        <v>97.2</v>
       </c>
       <c r="G112">
-        <v>98.4</v>
+        <v>89</v>
       </c>
       <c r="H112">
-        <v>48.2</v>
+        <v>30.7</v>
       </c>
       <c r="I112">
-        <v>32.6</v>
+        <v>30</v>
       </c>
       <c r="J112">
-        <v>21</v>
+        <v>24.4</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>2013</v>
+        <v>2010</v>
       </c>
       <c r="B113">
-        <v>1009.1</v>
+        <v>947.1</v>
       </c>
       <c r="C113">
         <v>1.7</v>
       </c>
       <c r="D113">
-        <v>290.3</v>
+        <v>279.7</v>
       </c>
       <c r="E113">
-        <v>156.5</v>
+        <v>149.80000000000001</v>
       </c>
       <c r="F113">
+        <v>97.7</v>
+      </c>
+      <c r="G113">
         <v>94.1</v>
       </c>
-      <c r="G113">
-        <v>97.8</v>
-      </c>
       <c r="H113">
-        <v>55.5</v>
+        <v>35.9</v>
       </c>
       <c r="I113">
-        <v>31.5</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="J113">
-        <v>20.7</v>
+        <v>23.4</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="B114">
-        <v>1014.9</v>
+        <v>993.1</v>
       </c>
       <c r="C114">
         <v>1.7</v>
       </c>
       <c r="D114">
-        <v>293.5</v>
+        <v>283.2</v>
       </c>
       <c r="E114">
-        <v>157</v>
+        <v>154.5</v>
       </c>
       <c r="F114">
-        <v>91.1</v>
+        <v>98.2</v>
       </c>
       <c r="G114">
-        <v>95.4</v>
+        <v>98.9</v>
       </c>
       <c r="H114">
-        <v>60.1</v>
+        <v>41.4</v>
       </c>
       <c r="I114">
-        <v>31.1</v>
+        <v>47.1</v>
       </c>
       <c r="J114">
-        <v>19.5</v>
+        <v>22.9</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="B115">
-        <v>1029.8</v>
+        <v>997.5</v>
       </c>
       <c r="C115">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="D115">
-        <v>295.5</v>
+        <v>286.60000000000002</v>
       </c>
       <c r="E115">
-        <v>156.5</v>
+        <v>157.9</v>
       </c>
       <c r="F115">
-        <v>89.4</v>
+        <v>96.5</v>
       </c>
       <c r="G115">
-        <v>96.5</v>
+        <v>98.4</v>
       </c>
       <c r="H115">
-        <v>67.7</v>
+        <v>48.2</v>
       </c>
       <c r="I115">
-        <v>30.6</v>
+        <v>32.6</v>
       </c>
       <c r="J115">
-        <v>18.5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116">
+        <v>2013</v>
+      </c>
+      <c r="B116">
+        <v>1009.1</v>
+      </c>
+      <c r="C116">
+        <v>1.7</v>
+      </c>
+      <c r="D116">
+        <v>290.3</v>
+      </c>
+      <c r="E116">
+        <v>156.5</v>
+      </c>
+      <c r="F116">
+        <v>94.1</v>
+      </c>
+      <c r="G116">
+        <v>97.8</v>
+      </c>
+      <c r="H116">
+        <v>55.5</v>
+      </c>
+      <c r="I116">
+        <v>31.5</v>
+      </c>
+      <c r="J116">
+        <v>20.7</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <v>2014</v>
+      </c>
+      <c r="B117">
+        <v>1014.9</v>
+      </c>
+      <c r="C117">
+        <v>1.7</v>
+      </c>
+      <c r="D117">
+        <v>293.5</v>
+      </c>
+      <c r="E117">
+        <v>157</v>
+      </c>
+      <c r="F117">
+        <v>91.1</v>
+      </c>
+      <c r="G117">
+        <v>95.4</v>
+      </c>
+      <c r="H117">
+        <v>60.1</v>
+      </c>
+      <c r="I117">
+        <v>31.1</v>
+      </c>
+      <c r="J117">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>2015</v>
+      </c>
+      <c r="B118">
+        <v>1029.8</v>
+      </c>
+      <c r="C118">
+        <v>1.6</v>
+      </c>
+      <c r="D118">
+        <v>295.5</v>
+      </c>
+      <c r="E118">
+        <v>156.5</v>
+      </c>
+      <c r="F118">
+        <v>89.4</v>
+      </c>
+      <c r="G118">
+        <v>96.5</v>
+      </c>
+      <c r="H118">
+        <v>67.7</v>
+      </c>
+      <c r="I118">
+        <v>30.6</v>
+      </c>
+      <c r="J118">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A119">
         <v>2016</v>
       </c>
-      <c r="B116">
+      <c r="B119">
         <v>1046.4000000000001</v>
       </c>
-      <c r="C116">
+      <c r="C119">
         <v>1.5</v>
       </c>
-      <c r="D116">
+      <c r="D119">
         <v>298.39999999999998</v>
       </c>
-      <c r="E116">
+      <c r="E119">
         <v>158.4</v>
       </c>
-      <c r="F116">
+      <c r="F119">
         <v>87.5</v>
       </c>
-      <c r="G116">
+      <c r="G119">
         <v>95.5</v>
       </c>
-      <c r="H116">
+      <c r="H119">
         <v>74.3</v>
       </c>
-      <c r="I116">
+      <c r="I119">
         <v>30.6</v>
       </c>
-      <c r="J116">
+      <c r="J119">
         <v>16.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
did EDA on each individual contextual data table, and merged into a singular one
</commit_message>
<xml_diff>
--- a/data/death_causes.xlsx
+++ b/data/death_causes.xlsx
@@ -78,9 +78,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>tuberculosis_deaths</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>deaths</t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -429,8 +429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="N110" sqref="N110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,34 +450,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>